<commit_message>
Adding more content and examples  to the API part of the workshop.
</commit_message>
<xml_diff>
--- a/data/Cyclanthaceae.xlsx
+++ b/data/Cyclanthaceae.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kimstp/Documents/NHMD/src/pythonprogramming/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B58B15CF-89F0-7B40-9BE0-8A4BD58B845A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0918B80-71FE-4748-AC6E-706B9078A3B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -728,7 +728,7 @@
   <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -737,6 +737,7 @@
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.83203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="21.5" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>